<commit_message>
IO Updates to model, updated with current US .mdl
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
+++ b/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\SoBCaICbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801A568A-4A9A-4A92-8DE0-40083EE19C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9DDD6A-EE2B-467B-813D-2B7069B42CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1290" windowWidth="24765" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="585" windowWidth="24090" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -45,6 +45,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="622">
   <si>
     <t>Notes</t>
   </si>
@@ -2193,12 +2194,6 @@
     <t>Other equipment includes primarily additional plug load equipment including computers and televisions</t>
   </si>
   <si>
-    <t>We assume all other equipment are direct purchase without install</t>
-  </si>
-  <si>
-    <t>Mostly likely to be TVs, computers, and monitors</t>
-  </si>
-  <si>
     <t>Note from "Updated Building Sector Appliance and Equipment Costs and Efficiencies."</t>
   </si>
   <si>
@@ -2212,6 +2207,18 @@
   </si>
   <si>
     <t>Unit: dimensionless (%)</t>
+  </si>
+  <si>
+    <t>We use the same breakdown as for appliances for</t>
+  </si>
+  <si>
+    <t>the other equipment category</t>
+  </si>
+  <si>
+    <t>ISIC 20</t>
+  </si>
+  <si>
+    <t>ISIC 21</t>
   </si>
 </sst>
 </file>
@@ -3341,7 +3348,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3456,17 +3463,17 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="114" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="113" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="113" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -3518,7 +3525,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3527,9 +3534,9 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -3559,88 +3566,91 @@
         <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>620</v>
       </c>
       <c r="L1" t="s">
+        <v>621</v>
+      </c>
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>61</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>67</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>68</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -3710,11 +3720,11 @@
       </c>
       <c r="R2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.54557663658145084</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.54557663658145084</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -3730,11 +3740,11 @@
       </c>
       <c r="W2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.45442336341854916</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.45442336341854916</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -3788,8 +3798,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -3859,11 +3873,11 @@
       </c>
       <c r="R3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.76199981922600579</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.76199981922600579</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -3879,11 +3893,11 @@
       </c>
       <c r="W3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.23800018077399421</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.23800018077399421</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -3937,8 +3951,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -4086,8 +4104,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -4153,11 +4175,11 @@
       </c>
       <c r="Q5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -4235,8 +4257,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -4302,11 +4328,11 @@
       </c>
       <c r="Q6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -4326,11 +4352,11 @@
       </c>
       <c r="W6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4384,8 +4410,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -4451,11 +4481,11 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -4479,7 +4509,7 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4531,6 +4561,10 @@
       </c>
       <c r="AK7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -4544,7 +4578,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4553,9 +4587,9 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -4585,88 +4619,91 @@
         <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>620</v>
       </c>
       <c r="L1" t="s">
+        <v>621</v>
+      </c>
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>61</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>67</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>68</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -4736,11 +4773,11 @@
       </c>
       <c r="R2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.70398750275034405</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.70398750275034405</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -4756,11 +4793,11 @@
       </c>
       <c r="W2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.29601249724965595</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.29601249724965595</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4814,8 +4851,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -4885,11 +4926,11 @@
       </c>
       <c r="R3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.5798301102469372</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.5798301102469372</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -4905,11 +4946,11 @@
       </c>
       <c r="W3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.4201698897530628</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.4201698897530628</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4963,8 +5004,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -5112,8 +5157,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -5179,11 +5228,11 @@
       </c>
       <c r="Q5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.40766894664785691</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.40766894664785691</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -5203,11 +5252,11 @@
       </c>
       <c r="W5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.59233105335214309</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.59233105335214309</v>
       </c>
       <c r="Y5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -5261,8 +5310,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -5328,11 +5381,11 @@
       </c>
       <c r="Q6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.75439886948727197</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.75439886948727197</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -5352,11 +5405,11 @@
       </c>
       <c r="W6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.24560113051272803</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.24560113051272803</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -5410,8 +5463,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -5477,11 +5534,11 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.75439886948727197</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -5505,7 +5562,7 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.24560113051272803</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -5557,6 +5614,10 @@
       </c>
       <c r="AK7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -35693,7 +35754,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35940,20 +36001,23 @@
         <v>2</v>
       </c>
       <c r="C11" s="105">
-        <v>1</v>
+        <f>C9</f>
+        <v>0.7542031594839681</v>
       </c>
       <c r="D11" s="105">
-        <v>1</v>
+        <f t="shared" ref="D11:E11" si="0">D9</f>
+        <v>0.7542031594839681</v>
       </c>
       <c r="E11" s="105">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.75439886948727197</v>
       </c>
       <c r="F11" s="106" t="str">
         <f>'ISIC Code Mapping'!G2</f>
         <v>ISIC 27</v>
       </c>
       <c r="G11" s="106" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -35964,20 +36028,23 @@
         <v>3</v>
       </c>
       <c r="C12" s="105">
-        <v>0</v>
+        <f>C10</f>
+        <v>0.2457968405160319</v>
       </c>
       <c r="D12" s="105">
-        <v>0</v>
+        <f t="shared" ref="D12:E12" si="1">D10</f>
+        <v>0.2457968405160319</v>
       </c>
       <c r="E12" s="105">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.24560113051272803</v>
       </c>
       <c r="F12" s="106" t="str">
         <f>'ISIC Code Mapping'!G3</f>
         <v>ISIC 41T43</v>
       </c>
       <c r="G12" s="106" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -36110,7 +36177,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -36119,9 +36186,9 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -36151,88 +36218,91 @@
         <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>620</v>
       </c>
       <c r="L1" t="s">
+        <v>621</v>
+      </c>
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>61</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>67</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>68</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -36302,11 +36372,11 @@
       </c>
       <c r="R2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.54557663658145084</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.54557663658145084</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -36322,11 +36392,11 @@
       </c>
       <c r="W2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.45442336341854916</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.45442336341854916</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -36380,8 +36450,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -36451,11 +36525,11 @@
       </c>
       <c r="R3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.76199981922600579</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.76199981922600579</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -36471,11 +36545,11 @@
       </c>
       <c r="W3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.23800018077399421</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.23800018077399421</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -36529,8 +36603,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -36678,8 +36756,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -36745,11 +36827,11 @@
       </c>
       <c r="Q5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -36827,8 +36909,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -36894,11 +36980,11 @@
       </c>
       <c r="Q6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -36918,11 +37004,11 @@
       </c>
       <c r="W6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -36976,8 +37062,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -37043,11 +37133,11 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -37071,7 +37161,7 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -37123,6 +37213,10 @@
       </c>
       <c r="AK7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to MN files - IO data, grid battery storage, MCGLT, other files w/ no value change - most recent Jun's export
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
+++ b/InputData/bldgs/SoBCaICbIC/Shr of Bldg Cap and Instl Costs by ISIC Code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\SoBCaICbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801A568A-4A9A-4A92-8DE0-40083EE19C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9DDD6A-EE2B-467B-813D-2B7069B42CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1290" windowWidth="24765" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="585" windowWidth="24090" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="4" r:id="rId1"/>
@@ -45,6 +45,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2715" uniqueCount="622">
   <si>
     <t>Notes</t>
   </si>
@@ -2193,12 +2194,6 @@
     <t>Other equipment includes primarily additional plug load equipment including computers and televisions</t>
   </si>
   <si>
-    <t>We assume all other equipment are direct purchase without install</t>
-  </si>
-  <si>
-    <t>Mostly likely to be TVs, computers, and monitors</t>
-  </si>
-  <si>
     <t>Note from "Updated Building Sector Appliance and Equipment Costs and Efficiencies."</t>
   </si>
   <si>
@@ -2212,6 +2207,18 @@
   </si>
   <si>
     <t>Unit: dimensionless (%)</t>
+  </si>
+  <si>
+    <t>We use the same breakdown as for appliances for</t>
+  </si>
+  <si>
+    <t>the other equipment category</t>
+  </si>
+  <si>
+    <t>ISIC 20</t>
+  </si>
+  <si>
+    <t>ISIC 21</t>
   </si>
 </sst>
 </file>
@@ -3341,7 +3348,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3456,17 +3463,17 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="114" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="113" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="113" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -3518,7 +3525,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3527,9 +3534,9 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -3559,88 +3566,91 @@
         <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>620</v>
       </c>
       <c r="L1" t="s">
+        <v>621</v>
+      </c>
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>61</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>67</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>68</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -3710,11 +3720,11 @@
       </c>
       <c r="R2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.54557663658145084</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.54557663658145084</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -3730,11 +3740,11 @@
       </c>
       <c r="W2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.45442336341854916</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.45442336341854916</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -3788,8 +3798,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -3859,11 +3873,11 @@
       </c>
       <c r="R3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.76199981922600579</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.76199981922600579</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -3879,11 +3893,11 @@
       </c>
       <c r="W3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.23800018077399421</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.23800018077399421</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -3937,8 +3951,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -4086,8 +4104,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -4153,11 +4175,11 @@
       </c>
       <c r="Q5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -4235,8 +4257,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -4302,11 +4328,11 @@
       </c>
       <c r="Q6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -4326,11 +4352,11 @@
       </c>
       <c r="W6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4384,8 +4410,12 @@
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -4451,11 +4481,11 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -4479,7 +4509,7 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4531,6 +4561,10 @@
       </c>
       <c r="AK7">
         <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <f>SUMIFS('Cost Breakdowns'!$D$3:$D$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -4544,7 +4578,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4553,9 +4587,9 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -4585,88 +4619,91 @@
         <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>620</v>
       </c>
       <c r="L1" t="s">
+        <v>621</v>
+      </c>
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>61</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>67</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>68</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -4736,11 +4773,11 @@
       </c>
       <c r="R2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.70398750275034405</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.70398750275034405</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -4756,11 +4793,11 @@
       </c>
       <c r="W2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.29601249724965595</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.29601249724965595</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4814,8 +4851,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -4885,11 +4926,11 @@
       </c>
       <c r="R3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.5798301102469372</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.5798301102469372</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -4905,11 +4946,11 @@
       </c>
       <c r="W3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.4201698897530628</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.4201698897530628</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -4963,8 +5004,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -5112,8 +5157,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -5179,11 +5228,11 @@
       </c>
       <c r="Q5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.40766894664785691</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.40766894664785691</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -5203,11 +5252,11 @@
       </c>
       <c r="W5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.59233105335214309</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.59233105335214309</v>
       </c>
       <c r="Y5">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -5261,8 +5310,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -5328,11 +5381,11 @@
       </c>
       <c r="Q6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.75439886948727197</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.75439886948727197</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -5352,11 +5405,11 @@
       </c>
       <c r="W6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.24560113051272803</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.24560113051272803</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -5410,8 +5463,12 @@
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -5477,11 +5534,11 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.75439886948727197</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -5505,7 +5562,7 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.24560113051272803</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -5557,6 +5614,10 @@
       </c>
       <c r="AK7">
         <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <f>SUMIFS('Cost Breakdowns'!$E$3:$E$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
     </row>
@@ -35693,7 +35754,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35940,20 +36001,23 @@
         <v>2</v>
       </c>
       <c r="C11" s="105">
-        <v>1</v>
+        <f>C9</f>
+        <v>0.7542031594839681</v>
       </c>
       <c r="D11" s="105">
-        <v>1</v>
+        <f t="shared" ref="D11:E11" si="0">D9</f>
+        <v>0.7542031594839681</v>
       </c>
       <c r="E11" s="105">
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>0.75439886948727197</v>
       </c>
       <c r="F11" s="106" t="str">
         <f>'ISIC Code Mapping'!G2</f>
         <v>ISIC 27</v>
       </c>
       <c r="G11" s="106" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -35964,20 +36028,23 @@
         <v>3</v>
       </c>
       <c r="C12" s="105">
-        <v>0</v>
+        <f>C10</f>
+        <v>0.2457968405160319</v>
       </c>
       <c r="D12" s="105">
-        <v>0</v>
+        <f t="shared" ref="D12:E12" si="1">D10</f>
+        <v>0.2457968405160319</v>
       </c>
       <c r="E12" s="105">
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>0.24560113051272803</v>
       </c>
       <c r="F12" s="106" t="str">
         <f>'ISIC Code Mapping'!G3</f>
         <v>ISIC 41T43</v>
       </c>
       <c r="G12" s="106" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -36110,7 +36177,7 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -36119,9 +36186,9 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="99" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="B1" t="s">
         <v>40</v>
@@ -36151,88 +36218,91 @@
         <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>620</v>
       </c>
       <c r="L1" t="s">
+        <v>621</v>
+      </c>
+      <c r="M1" t="s">
         <v>50</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>52</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>53</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>56</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>57</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>58</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>59</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>60</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>61</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>62</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>65</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>66</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>67</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>68</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>69</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>70</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>71</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>72</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>73</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>74</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>492</v>
       </c>
@@ -36302,11 +36372,11 @@
       </c>
       <c r="R2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.54557663658145084</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.54557663658145084</v>
       </c>
       <c r="T2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -36322,11 +36392,11 @@
       </c>
       <c r="W2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.45442336341854916</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.45442336341854916</v>
       </c>
       <c r="Y2">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -36380,8 +36450,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL2">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A2,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="64" t="s">
         <v>493</v>
       </c>
@@ -36451,11 +36525,11 @@
       </c>
       <c r="R3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0.76199981922600579</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
-        <v>0</v>
+        <v>0.76199981922600579</v>
       </c>
       <c r="T3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!T$1)</f>
@@ -36471,11 +36545,11 @@
       </c>
       <c r="W3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.23800018077399421</v>
+        <v>0</v>
       </c>
       <c r="X3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.23800018077399421</v>
       </c>
       <c r="Y3">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -36529,8 +36603,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL3">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A3,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
         <v>605</v>
       </c>
@@ -36678,8 +36756,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL4">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A4,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="64" t="s">
         <v>499</v>
       </c>
@@ -36745,11 +36827,11 @@
       </c>
       <c r="Q5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -36827,8 +36909,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL5">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A5,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="64" t="s">
         <v>561</v>
       </c>
@@ -36894,11 +36980,11 @@
       </c>
       <c r="Q6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>0.7542031594839681</v>
+        <v>0</v>
       </c>
       <c r="R6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -36918,11 +37004,11 @@
       </c>
       <c r="W6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!W$1)</f>
-        <v>0.2457968405160319</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y6">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -36976,8 +37062,12 @@
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL6">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A6,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
         <v>82</v>
       </c>
@@ -37043,11 +37133,11 @@
       </c>
       <c r="Q7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Q$1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!R$1)</f>
-        <v>0</v>
+        <v>0.7542031594839681</v>
       </c>
       <c r="S7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!S$1)</f>
@@ -37071,7 +37161,7 @@
       </c>
       <c r="X7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!X$1)</f>
-        <v>0</v>
+        <v>0.2457968405160319</v>
       </c>
       <c r="Y7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!Y$1)</f>
@@ -37123,6 +37213,10 @@
       </c>
       <c r="AK7">
         <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AK$1)</f>
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <f>SUMIFS('Cost Breakdowns'!$C$3:$C$12,'Cost Breakdowns'!$A$3:$A$12,'SoBCaICbIC-urbanresidential'!$A7,'Cost Breakdowns'!$F$3:$F$12,'SoBCaICbIC-urbanresidential'!AL$1)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>